<commit_message>
Build infrastructure for text display; change outputs to be compatible with code portfolio standards
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/travel_weather/A_Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DFE617-3203-7F45-A3DD-B07BD16ECBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B413607E-1851-4445-B105-41B491D9EE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34380" yWindow="900" windowWidth="20620" windowHeight="14260" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-34280" yWindow="2120" windowWidth="23380" windowHeight="15340" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="286">
   <si>
     <t>Num</t>
   </si>
@@ -759,157 +759,145 @@
     <t>Dec</t>
   </si>
   <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>best_temp_1</t>
+  </si>
+  <si>
+    <t>best_temp_2</t>
+  </si>
+  <si>
+    <t>bt1</t>
+  </si>
+  <si>
+    <t>bt2</t>
+  </si>
+  <si>
+    <t>states_etc</t>
+  </si>
+  <si>
+    <t>url1</t>
+  </si>
+  <si>
+    <t>url2</t>
+  </si>
+  <si>
+    <t>url3</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Toronto,+ON,+Canada/Ottawa,+ON,+Canada/Montreal,+QC,+Canada/Qu%C3%A9bec,+QC,+Canada/Montr%C3%A9al,+QC,+Canada/Toronto,+ON,+Canada/@45.1540678,-79.7807285,6z/data=!3m1!4b1!4m41!4m40!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!1m5!1m1!1s0x4cce05b25f5113af:0x8a6a51e131dd15ed!2m2!1d-75.6971931!2d45.4215296!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x4cb8968a05db8893:0x8fc52d63f0e83a03!2m2!1d-71.2079809!2d46.8138783!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Anchorage,+AK/Fairbanks,+AK/Anchorage,+AK/@63.8441792,-152.4627417,6.14z/data=!4m22!4m21!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!1m5!1m1!1s0x5132454f67fd65a9:0xb3d805e009fef73a!2m2!1d-147.7163888!2d64.8377778!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!2m1!2b1!3e0</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Denver,+CO/Grand+Junction,+CO/Salt+Lake+City,+UT/Boise,+ID/Idaho+Falls,+ID/Helena,+MT/Billings,+MT/Casper,+WY/Cheyenne,+WY/Denver,+Colorado/@42.4201276,-119.4822548,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!1m5!1m1!1s0x8746d6e322e77057:0xcc63f451cebf7c56!2m2!1d-108.5506486!2d39.0638705!1m5!1m1!1s0x87523d9488d131ed:0x5b53b7a0484d31ca!2m2!1d-111.8910474!2d40.7607793!1m5!1m1!1s0x54aef172e947b49d:0x9a5b989b36679d9b!2m2!1d-116.2023137!2d43.6150186!1m5!1m1!1s0x5354594e739512b5:0x2311c9fc094c49c9!2m2!1d-112.0407584!2d43.4926607!1m5!1m1!1s0x5343510fedc7db4d:0x214c1d71e3fdf714!2m2!1d-112.0391057!2d46.5891452!1m5!1m1!1s0x53486f8888fa9d97:0x373556d4f179b550!2m2!1d-108.5006904!2d45.7832856!1m5!1m1!1s0x87609365c85e7a63:0x69cefc3917343e53!2m2!1d-106.2980824!2d42.848709!1m5!1m1!1s0x876f38762e73ef93:0xb10a30418f972d2b!2m2!1d-104.8202462!2d41.1399814!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Minneapolis,+MN/Sioux+Falls,+SD/Pierre,+SD/Bismarck,+ND/Fargo,+ND/Winnipeg,+MB,+Canada/Duluth,+MN/Minneapolis,+MN/@46.6404497,-100.928197,6z/data=!3m1!4b1!4m53!4m52!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!1m5!1m1!1s0x878eb498e0bdacd7:0xde95ff3aa8b2fccf!2m2!1d-96.731265!2d43.5460223!1m5!1m1!1s0x52d54a64b288f891:0x9e9950165931af92!2m2!1d-100.3537522!2d44.3667876!1m5!1m1!1s0x52d7831257d8e963:0xccaabd12f9bbca93!2m2!1d-100.7837392!2d46.8083268!1m5!1m1!1s0x52c8cb8d84677145:0x81aa30a52791aaca!2m2!1d-96.7898034!2d46.8771863!1m5!1m1!1s0x52ea73fbf91a2b11:0x2b2a1afac6b9ca64!2m2!1d-97.1383744!2d49.895136!1m5!1m1!1s0x52ae527e782e37ff:0x90fdbf76eb580c72!2m2!1d-92.1004852!2d46.7866719!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Seattle,+WA/Vancouver,+BC,+Canada/Leavenworth,+WA/Spokane,+WA/Redding,+CA/Gold+Beach,+OR/Salem,+OR/Portland,+OR/Olympia,+WA/Seattle,+WA/@44.8374018,-125.1438928,6.26z/data=!4m65!4m64!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!1m5!1m1!1s0x548673f143a94fb3:0xbb9196ea9b81f38b!2m2!1d-123.1207375!2d49.2827291!1m5!1m1!1s0x549a4d92a4f8f98d:0xa14f95fb0abfef7e!2m2!1d-120.6614765!2d47.5962326!1m5!1m1!1s0x549e185c30bbe7e5:0xddfcc9d60b84d9b1!2m2!1d-117.4260465!2d47.6587802!1m5!1m1!1s0x54d291d63b4a202f:0x1f3358ec7b360f57!2m2!1d-122.3916754!2d40.5865396!1m5!1m1!1s0x54dace49bf9ae73d:0x121195079f68806d!2m2!1d-124.4217741!2d42.4073334!1m5!1m1!1s0x54bffefcbc4b9c63:0xf93429e08f0357c2!2m2!1d-123.0350963!2d44.9428975!1m5!1m1!1s0x54950b0b7da97427:0x1c36b9e6f6d18591!2m2!1d-122.6783853!2d45.515232!1m5!1m1!1s0x5491c9c1ae285569:0x4f146197e2881b83!2m2!1d-122.9006951!2d47.0378741!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Albany,+NY/Burlington,+VT/Montpelier,+VT/Concord,+NH/Augusta,+ME/Portland,+ME/Boston,+MA/Barnstable,+MA/Providence,+RI/Hartford,+CT/@41.8793352,-74.5474305,7z/data=!4m65!4m64!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!1m5!1m1!1s0x4cca7a55b69b55e5:0xc35fe519720e498e!2m2!1d-73.212072!2d44.4758825!1m5!1m1!1s0x4cb5a78cc44dea05:0x4891e094ceb5836!2m2!1d-72.5753869!2d44.2600593!1m5!1m1!1s0x89e26a96154a8917:0x5a871a0a62528f1!2m2!1d-71.5375718!2d43.2081366!1m5!1m1!1s0x4cb200fdafacc49d:0x79a3488d64220b2d!2m2!1d-69.7794897!2d44.3106241!1m5!1m1!1s0x4cb29c72aab0ee2d:0x7e9db6b53372fa29!2m2!1d-70.2568189!2d43.6590993!1m5!1m1!1s0x89e3652d0d3d311b:0x787cbf240162e8a0!2m2!1d-71.0588801!2d42.3600825!1m5!1m1!1s0x89fb33b67f8ec5e5:0xea7648efbb136d73!2m2!1d-70.3002024!2d41.7003208!1m5!1m1!1s0x89e444e0437e735d:0x69df7c4d48b3b627!2m2!1d-71.4128343!2d41.8239891!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Hartford,+CT/New+York,+NY/Trenton,+NJ/Philadelphia,+PA/Dover,+DE/Annapolis,+MD/Baltimore,+MD/Washington+D.C.,+DC/Richmond,+VA/Williamsburg,+VA/@39.5003974,-77.3244192,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!1m5!1m1!1s0x89c24fa5d33f083b:0xc80b8f06e177fe62!2m2!1d-74.0059728!2d40.7127753!1m5!1m1!1s0x89c143482d3dbbb9:0xcf16567f895cd7bc!2m2!1d-74.759717!2d40.2205824!1m5!1m1!1s0x89c6b7d8d4b54beb:0x89f514d88c3e58c1!2m2!1d-75.1652215!2d39.9525839!1m5!1m1!1s0x89c7633375685ead:0xa9e2e447fb006cf0!2m2!1d-75.5243682!2d39.158168!1m5!1m1!1s0x89b7f66570672fd5:0x43f854fdd3a8274b!2m2!1d-76.4921829!2d38.9784453!1m5!1m1!1s0x89c803aed6f483b7:0x44896a84223e758!2m2!1d-76.6121893!2d39.2903848!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x89b111095799c9ed:0xbfd83e6de2423cc5!2m2!1d-77.4360481!2d37.5407246!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Williamsburg,+VA/Norfolk,+VA/Charlottesville,+VA/Harrisburg,+PA/Buffalo,+NY/Rochester,+NY/Albany,+NY/@40.2169587,-81.2677638,5.7z/data=!4m47!4m46!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!1m5!1m1!1s0x89ba973a5322ca45:0xab99107fce7a1e0a!2m2!1d-76.2858726!2d36.8507689!1m5!1m1!1s0x89b3862dea50a48f:0x9086f096c38b74fc!2m2!1d-78.4766781!2d38.0293059!1m5!1m1!1s0x89c8c116b8079e97:0xbb6e42c8128d46d5!2m2!1d-76.8867008!2d40.2731911!1m5!1m1!1s0x89d3126152dfe5a1:0x982304a5181f8171!2m2!1d-78.8783689!2d42.8864468!1m5!1m1!1s0x89d6b3059614b353:0x5a001ffc4125e61e!2m2!1d-77.6088465!2d43.1565779!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Pittsburgh,+PA/Charleston,+WV/Columbus,+OH/Cincinnati,+OH/Frankfort,+KY/Louisville,+KY/Indianapolis,+IN/Chicago,+IL/Milwaukee,+WI/Madison,+WI/@40.5504662,-89.1782838,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!1m5!1m1!1s0x884f2cce88145d39:0x7661a84704c91b0b!2m2!1d-81.6326234!2d38.3498195!1m5!1m1!1s0x883889c1b990de71:0xe43266f8cfb1b533!2m2!1d-82.9987942!2d39.9611755!1m5!1m1!1s0x884051b1de3821f9:0x69fb7e8be4c09317!2m2!1d-84.5120196!2d39.1031182!1m5!1m1!1s0x8842734c8b1953c9:0x536418a08867425c!2m2!1d-84.8732835!2d38.2009055!1m5!1m1!1s0x88690b1ab35bd511:0xd4d3b4282071fd32!2m2!1d-85.7584557!2d38.2526647!1m5!1m1!1s0x886b50ffa7796a03:0xd68e9df640b9ea7c!2m2!1d-86.158068!2d39.768403!1m5!1m1!1s0x880e2c3cd0f4cbed:0xafe0a6ad09c0c000!2m2!1d-87.6297982!2d41.8781136!1m5!1m1!1s0x880502d7578b47e7:0x445f1922b5417b84!2m2!1d-87.9064736!2d43.0389025!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Madison,+Wisconsin/Green+Bay,+WI/Mackinaw+City,+MI/Grand+Rapids,+MI/Lansing,+MI/Frankenmuth,+MI/Detroit,+MI/Cleveland,+OH/Pittsburgh,+PA/@43.1918863,-89.1853954,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!1m5!1m1!1s0x8802e2e809b380f3:0x6370045214dcf571!2m2!1d-88.0132958!2d44.5133188!1m5!1m1!1s0x4d358b3940a9ad83:0xeac771ab20cc7a7a!2m2!1d-84.7271465!2d45.7774987!1m5!1m1!1s0x88185460bb502815:0xa593aacb1bd3a8d0!2m2!1d-85.6680863!2d42.9633599!1m5!1m1!1s0x8822c01c7f318c37:0x4378b62389029d9e!2m2!1d-84.5555347!2d42.732535!1m5!1m1!1s0x8823f287285df793:0x8050516199bcb01f!2m2!1d-83.7380194!2d43.331691!1m5!1m1!1s0x8824ca0110cb1d75:0x5776864e35b9c4d2!2m2!1d-83.0457538!2d42.331427!1m5!1m1!1s0x8830ef2ee3686b2d:0xed04cb55f7621842!2m2!1d-81.6943605!2d41.49932!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/San+Juan,+Puerto+Rico/@28.406847,-80.5870322,5z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x8c03686fe268196f:0xad6b7f0f5c935adc!2m2!1d-66.1057355!2d18.4655394!3e4</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/Honolulu,+HI/@24.8112769,-154.8564566,3z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x7c00183b8cc3464d:0x4b28f55ff3a7976c!2m2!1d-157.8583333!2d21.3069444!3e4</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Orlando,+FL/Miami,+FL/Key+West,+FL/Everglades+City,+FL/Tampa,+FL/Tarpon+Springs,+FL/Tallahassee,+FL/Jacksonville,+FL/St.+Augustine,+FL/Orlando,+FL/@27.5091232,-84.4177219,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!1m5!1m1!1s0x88d9b0a20ec8c111:0xff96f271ddad4f65!2m2!1d-80.1917902!2d25.7616798!1m5!1m1!1s0x88d1b134ad952377:0x3fcee92f77463b5e!2m2!1d-81.7799871!2d24.5550593!1m5!1m1!1s0x88da5c605ba45fb1:0x92bcf49fb504533a!2m2!1d-81.3850695!2d25.8582443!1m5!1m1!1s0x88c2b782b3b9d1e1:0xa75f1389af96b463!2m2!1d-82.4571776!2d27.950575!1m5!1m1!1s0x88c28cfd6f0942df:0xf4297f0ce0bf24b7!2m2!1d-82.7567679!2d28.1461248!1m5!1m1!1s0x88ec8a5187124b53:0xebee077ad4fdb1f8!2m2!1d-84.2807329!2d30.4382559!1m5!1m1!1s0x88e5b716f1ceafeb:0xc4cd7d3896fcc7e2!2m2!1d-81.655651!2d30.3321838!1m5!1m1!1s0x88e6825775df7f4f:0xc2a183178b276027!2m2!1d-81.3124341!2d29.9012437!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Los+Angeles,+CA/Santa+Barbara,+CA/Solvang,+CA/San+Jose,+CA/San+Francisco,+CA/Sacramento,+CA/Reno,+NV/Virginia+City,+NV/Carson+City,+NV/Fresno,+CA/@36.7777641,-122.6363689,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!1m5!1m1!1s0x80e914c76f2d83d5:0xc8d13a64d7ba7648!2m2!1d-119.6981901!2d34.4208305!1m5!1m1!1s0x80e954a0fc922285:0x2d0e281b060bc156!2m2!1d-120.1376481!2d34.5958201!1m5!1m1!1s0x808fcae48af93ff5:0xb99d8c0aca9f717b!2m2!1d-121.8863286!2d37.3382082!1m5!1m1!1s0x80859a6d00690021:0x4a501367f076adff!2m2!1d-122.4194155!2d37.7749295!1m5!1m1!1s0x809ac672b28397f9:0x921f6aaa74197fdb!2m2!1d-121.4943996!2d38.5815719!1m5!1m1!1s0x809940ae9292a09d:0x40c5c5ce7438f787!2m2!1d-119.8138027!2d39.5296329!1m5!1m1!1s0x80990faad3daafd1:0x29dad257dc576fa9!2m2!1d-119.6499793!2d39.3095135!1m5!1m1!1s0x80990aa1f8deb471:0xf79c6c82bde23828!2m2!1d-119.7674034!2d39.1637984!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Fresno,+CA/Riverside,+CA/San+Diego,+CA/Los+Angeles,+CA/@34.7127545,-120.6716835,7z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!1m5!1m1!1s0x80dca6df7ff47dbb:0xf7a1d705135e0ae8!2m2!1d-117.3754942!2d33.9806005!1m5!1m1!1s0x80d9530fad921e4b:0xd3a21fdfd15df79!2m2!1d-117.1610838!2d32.715738!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Phoenix,+AZ/Sedona,+AZ/Las+Vegas,+NV/St.+George,+UT/Taos,+NM/Santa+Fe,+NM/Albuquerque,+NM/Lubbock,+TX/El+Paso,+TX/Tucson,+AZ/@34.1501088,-117.508012,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!1m5!1m1!1s0x872da132f942b00d:0x5548c523fa6c8efd!2m2!1d-111.7609896!2d34.8697395!1m5!1m1!1s0x80beb782a4f57dd1:0x3accd5e6d5b379a3!2m2!1d-115.1398296!2d36.1699412!1m5!1m1!1s0x80ca44d0984939e5:0x531707f2f8a11c1e!2m2!1d-113.5684164!2d37.0965278!1m5!1m1!1s0x871764da7f11fcb1:0x90ea918361a9b782!2m2!1d-105.5733788!2d36.4072134!1m5!1m1!1s0x87185043e79852a9:0x8c902373fd88df40!2m2!1d-105.937799!2d35.6869752!1m5!1m1!1s0x87220addd309837b:0xc0d3f8ceb8d9f6fd!2m2!1d-106.650422!2d35.0843859!1m5!1m1!1s0x86fe12add37ddd39:0x1af0042922e84287!2m2!1d-101.8551665!2d33.5778631!1m5!1m1!1s0x86e73f8bc5fe3b69:0xe39184e3ab9d0222!2m2!1d-106.4850217!2d31.7618778!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Tucson,+AZ/Phoenix,+AZ/@32.6659365,-112.3105217,7.68z/data=!4m17!4m16!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Dallas,+TX/Austin,+TX/San+Antonio,+TX/McAllen,+TX/Houston,+TX/Baton+Rouge,+LA/New+Orleans,+LA/Gulfport,+MS/Jackson,+MS/@29.4197283,-98.2903561,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!1m5!1m1!1s0x8644b599a0cc032f:0x5d9b464bd469d57a!2m2!1d-97.7430608!2d30.267153!1m5!1m1!1s0x865c58af04d00eaf:0x856e13b10a016bc!2m2!1d-98.4936282!2d29.4241219!1m5!1m1!1s0x866576324d9637df:0x2f1d39a9b52c0eb8!2m2!1d-98.2300124!2d26.2034071!1m5!1m1!1s0x8640b8b4488d8501:0xca0d02def365053b!2m2!1d-95.3698028!2d29.7604267!1m5!1m1!1s0x86243867325f74cb:0x2123f1db91579a1d!2m2!1d-91.1871466!2d30.4514677!1m5!1m1!1s0x8620a454b2118265:0xdb065be85e22d3b4!2m2!1d-90.0715323!2d29.9510658!1m5!1m1!1s0x889c166ee80114e5:0xc2614d446e819544!2m2!1d-89.0928155!2d30.3674198!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Jackson,+MS/Little+Rock,+AR/Fayetteville,+AR/Dallas,+TX/@32.5477822,-99.0081422,5.75z/data=!4m29!4m28!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!1m5!1m1!1s0x87d2a134a11f569b:0x3405f5100df35b17!2m2!1d-92.2895948!2d34.7464809!1m5!1m1!1s0x87c96f7b2fb53e9d:0x4519f069fcb4c8cf!2m2!1d-94.157853!2d36.0662419!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Atlanta,+GA/Helen,+GA/Nashville,+TN/Knoxville,+TN/Charlotte,+NC/Greensboro,+NC/Raleigh,+NC/Columbia,+SC/Charleston,+SC/Savannah,+GA/@34.0640266,-87.1468938,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!1m5!1m1!1s0x885f37d40b3a2aa1:0x8ed537fed96523a8!2m2!1d-83.7315675!2d34.7014839!1m5!1m1!1s0x8864ec3213eb903d:0x7d3fb9d0a1e9daa0!2m2!1d-86.7816016!2d36.1626638!1m5!1m1!1s0x885c162246ce42a9:0x7bea92dac4f534c5!2m2!1d-83.9207392!2d35.9606384!1m5!1m1!1s0x88541fc4fc381a81:0x884650e6bf43d164!2m2!1d-80.8431267!2d35.2270869!1m5!1m1!1s0x8853193f38c77b79:0x93b9c49478be12c8!2m2!1d-79.7919754!2d36.0726354!1m5!1m1!1s0x89ac5a2f9f51e0f7:0x6790b6528a11f0ad!2m2!1d-78.6381787!2d35.7795897!1m5!1m1!1s0x88f8a5697931d1e3:0xf32808f4b379fa96!2m2!1d-81.0348144!2d34.0007104!1m5!1m1!1s0x88fe7a42dca82477:0x35faf7e0aee1ec6b!2m2!1d-79.9310512!2d32.7764749!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/Savannah,+GA/Montgomery,+AL/Birmingham,+AL/Atlanta,+GA/@32.8510822,-88.4506539,6z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!1m5!1m1!1s0x888e8194b0d481f9:0x8e1b511d354285ff!2m2!1d-86.3077368!2d32.3792233!1m5!1m1!1s0x888911df5885bfd3:0x25507409eaba54ce!2m2!1d-86.8103567!2d33.5185892!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!2m1!2b1!3e0!4e1</t>
+  </si>
+  <si>
+    <t>Northeast + MD, DE, VA</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>SEA &gt; ANC</t>
+  </si>
+  <si>
+    <t>SFO &gt; HNL</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>old_order</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
     <t>Apr</t>
   </si>
   <si>
-    <t>Oct</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
-    <t>Sep</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>best_temp_1</t>
-  </si>
-  <si>
-    <t>best_temp_2</t>
-  </si>
-  <si>
-    <t>Aug-Sep</t>
-  </si>
-  <si>
-    <t>Oct-Nov</t>
-  </si>
-  <si>
-    <t>Nov-Dec</t>
-  </si>
-  <si>
-    <t>Jul-Aug</t>
-  </si>
-  <si>
-    <t>May-Jun</t>
-  </si>
-  <si>
-    <t>Apr-May</t>
-  </si>
-  <si>
-    <t>Mar-Apr</t>
-  </si>
-  <si>
-    <t>Jan-Mar</t>
-  </si>
-  <si>
-    <t>Jan-Feb</t>
-  </si>
-  <si>
-    <t>bt1</t>
-  </si>
-  <si>
-    <t>bt2</t>
-  </si>
-  <si>
-    <t>states_etc</t>
-  </si>
-  <si>
-    <t>url1</t>
-  </si>
-  <si>
-    <t>url2</t>
-  </si>
-  <si>
-    <t>url3</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Toronto,+ON,+Canada/Ottawa,+ON,+Canada/Montreal,+QC,+Canada/Qu%C3%A9bec,+QC,+Canada/Montr%C3%A9al,+QC,+Canada/Toronto,+ON,+Canada/@45.1540678,-79.7807285,6z/data=!3m1!4b1!4m41!4m40!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!1m5!1m1!1s0x4cce05b25f5113af:0x8a6a51e131dd15ed!2m2!1d-75.6971931!2d45.4215296!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x4cb8968a05db8893:0x8fc52d63f0e83a03!2m2!1d-71.2079809!2d46.8138783!1m5!1m1!1s0x4cc91a541c64b70d:0x654e3138211fefef!2m2!1d-73.567256!2d45.5016889!1m5!1m1!1s0x89d4cb90d7c63ba5:0x323555502ab4c477!2m2!1d-79.3831843!2d43.653226!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Anchorage,+AK/Fairbanks,+AK/Anchorage,+AK/@63.8441792,-152.4627417,6.14z/data=!4m22!4m21!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!1m5!1m1!1s0x5132454f67fd65a9:0xb3d805e009fef73a!2m2!1d-147.7163888!2d64.8377778!1m5!1m1!1s0x56c8917604b33f41:0x257dba5aa78468e3!2m2!1d-149.9002778!2d61.2180556!2m1!2b1!3e0</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Denver,+CO/Grand+Junction,+CO/Salt+Lake+City,+UT/Boise,+ID/Idaho+Falls,+ID/Helena,+MT/Billings,+MT/Casper,+WY/Cheyenne,+WY/Denver,+Colorado/@42.4201276,-119.4822548,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!1m5!1m1!1s0x8746d6e322e77057:0xcc63f451cebf7c56!2m2!1d-108.5506486!2d39.0638705!1m5!1m1!1s0x87523d9488d131ed:0x5b53b7a0484d31ca!2m2!1d-111.8910474!2d40.7607793!1m5!1m1!1s0x54aef172e947b49d:0x9a5b989b36679d9b!2m2!1d-116.2023137!2d43.6150186!1m5!1m1!1s0x5354594e739512b5:0x2311c9fc094c49c9!2m2!1d-112.0407584!2d43.4926607!1m5!1m1!1s0x5343510fedc7db4d:0x214c1d71e3fdf714!2m2!1d-112.0391057!2d46.5891452!1m5!1m1!1s0x53486f8888fa9d97:0x373556d4f179b550!2m2!1d-108.5006904!2d45.7832856!1m5!1m1!1s0x87609365c85e7a63:0x69cefc3917343e53!2m2!1d-106.2980824!2d42.848709!1m5!1m1!1s0x876f38762e73ef93:0xb10a30418f972d2b!2m2!1d-104.8202462!2d41.1399814!1m5!1m1!1s0x876b80aa231f17cf:0x118ef4f8278a36d6!2m2!1d-104.990251!2d39.7392358!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Minneapolis,+MN/Sioux+Falls,+SD/Pierre,+SD/Bismarck,+ND/Fargo,+ND/Winnipeg,+MB,+Canada/Duluth,+MN/Minneapolis,+MN/@46.6404497,-100.928197,6z/data=!3m1!4b1!4m53!4m52!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!1m5!1m1!1s0x878eb498e0bdacd7:0xde95ff3aa8b2fccf!2m2!1d-96.731265!2d43.5460223!1m5!1m1!1s0x52d54a64b288f891:0x9e9950165931af92!2m2!1d-100.3537522!2d44.3667876!1m5!1m1!1s0x52d7831257d8e963:0xccaabd12f9bbca93!2m2!1d-100.7837392!2d46.8083268!1m5!1m1!1s0x52c8cb8d84677145:0x81aa30a52791aaca!2m2!1d-96.7898034!2d46.8771863!1m5!1m1!1s0x52ea73fbf91a2b11:0x2b2a1afac6b9ca64!2m2!1d-97.1383744!2d49.895136!1m5!1m1!1s0x52ae527e782e37ff:0x90fdbf76eb580c72!2m2!1d-92.1004852!2d46.7866719!1m5!1m1!1s0x52b333909377bbbd:0x939fc9842f7aee07!2m2!1d-93.2650108!2d44.977753!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Seattle,+WA/Vancouver,+BC,+Canada/Leavenworth,+WA/Spokane,+WA/Redding,+CA/Gold+Beach,+OR/Salem,+OR/Portland,+OR/Olympia,+WA/Seattle,+WA/@44.8374018,-125.1438928,6.26z/data=!4m65!4m64!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!1m5!1m1!1s0x548673f143a94fb3:0xbb9196ea9b81f38b!2m2!1d-123.1207375!2d49.2827291!1m5!1m1!1s0x549a4d92a4f8f98d:0xa14f95fb0abfef7e!2m2!1d-120.6614765!2d47.5962326!1m5!1m1!1s0x549e185c30bbe7e5:0xddfcc9d60b84d9b1!2m2!1d-117.4260465!2d47.6587802!1m5!1m1!1s0x54d291d63b4a202f:0x1f3358ec7b360f57!2m2!1d-122.3916754!2d40.5865396!1m5!1m1!1s0x54dace49bf9ae73d:0x121195079f68806d!2m2!1d-124.4217741!2d42.4073334!1m5!1m1!1s0x54bffefcbc4b9c63:0xf93429e08f0357c2!2m2!1d-123.0350963!2d44.9428975!1m5!1m1!1s0x54950b0b7da97427:0x1c36b9e6f6d18591!2m2!1d-122.6783853!2d45.515232!1m5!1m1!1s0x5491c9c1ae285569:0x4f146197e2881b83!2m2!1d-122.9006951!2d47.0378741!1m5!1m1!1s0x5490102c93e83355:0x102565466944d59a!2m2!1d-122.3320708!2d47.6062095!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Albany,+NY/Burlington,+VT/Montpelier,+VT/Concord,+NH/Augusta,+ME/Portland,+ME/Boston,+MA/Barnstable,+MA/Providence,+RI/Hartford,+CT/@41.8793352,-74.5474305,7z/data=!4m65!4m64!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!1m5!1m1!1s0x4cca7a55b69b55e5:0xc35fe519720e498e!2m2!1d-73.212072!2d44.4758825!1m5!1m1!1s0x4cb5a78cc44dea05:0x4891e094ceb5836!2m2!1d-72.5753869!2d44.2600593!1m5!1m1!1s0x89e26a96154a8917:0x5a871a0a62528f1!2m2!1d-71.5375718!2d43.2081366!1m5!1m1!1s0x4cb200fdafacc49d:0x79a3488d64220b2d!2m2!1d-69.7794897!2d44.3106241!1m5!1m1!1s0x4cb29c72aab0ee2d:0x7e9db6b53372fa29!2m2!1d-70.2568189!2d43.6590993!1m5!1m1!1s0x89e3652d0d3d311b:0x787cbf240162e8a0!2m2!1d-71.0588801!2d42.3600825!1m5!1m1!1s0x89fb33b67f8ec5e5:0xea7648efbb136d73!2m2!1d-70.3002024!2d41.7003208!1m5!1m1!1s0x89e444e0437e735d:0x69df7c4d48b3b627!2m2!1d-71.4128343!2d41.8239891!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Hartford,+CT/New+York,+NY/Trenton,+NJ/Philadelphia,+PA/Dover,+DE/Annapolis,+MD/Baltimore,+MD/Washington+D.C.,+DC/Richmond,+VA/Williamsburg,+VA/@39.5003974,-77.3244192,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x89e65311f21151a5:0xcc8e4aa8e97d5999!2m2!1d-72.6733723!2d41.7658043!1m5!1m1!1s0x89c24fa5d33f083b:0xc80b8f06e177fe62!2m2!1d-74.0059728!2d40.7127753!1m5!1m1!1s0x89c143482d3dbbb9:0xcf16567f895cd7bc!2m2!1d-74.759717!2d40.2205824!1m5!1m1!1s0x89c6b7d8d4b54beb:0x89f514d88c3e58c1!2m2!1d-75.1652215!2d39.9525839!1m5!1m1!1s0x89c7633375685ead:0xa9e2e447fb006cf0!2m2!1d-75.5243682!2d39.158168!1m5!1m1!1s0x89b7f66570672fd5:0x43f854fdd3a8274b!2m2!1d-76.4921829!2d38.9784453!1m5!1m1!1s0x89c803aed6f483b7:0x44896a84223e758!2m2!1d-76.6121893!2d39.2903848!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x89b111095799c9ed:0xbfd83e6de2423cc5!2m2!1d-77.4360481!2d37.5407246!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Williamsburg,+VA/Norfolk,+VA/Charlottesville,+VA/Harrisburg,+PA/Buffalo,+NY/Rochester,+NY/Albany,+NY/@40.2169587,-81.2677638,5.7z/data=!4m47!4m46!1m5!1m1!1s0x89b0890a4495aa1b:0xc14b30175e160eaa!2m2!1d-76.7074571!2d37.2707022!1m5!1m1!1s0x89ba973a5322ca45:0xab99107fce7a1e0a!2m2!1d-76.2858726!2d36.8507689!1m5!1m1!1s0x89b3862dea50a48f:0x9086f096c38b74fc!2m2!1d-78.4766781!2d38.0293059!1m5!1m1!1s0x89c8c116b8079e97:0xbb6e42c8128d46d5!2m2!1d-76.8867008!2d40.2731911!1m5!1m1!1s0x89d3126152dfe5a1:0x982304a5181f8171!2m2!1d-78.8783689!2d42.8864468!1m5!1m1!1s0x89d6b3059614b353:0x5a001ffc4125e61e!2m2!1d-77.6088465!2d43.1565779!1m5!1m1!1s0x89de0a34cc4ffb4b:0xe1a16312a0e728c4!2m2!1d-73.7562317!2d42.6525793!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Pittsburgh,+PA/Charleston,+WV/Columbus,+OH/Cincinnati,+OH/Frankfort,+KY/Louisville,+KY/Indianapolis,+IN/Chicago,+IL/Milwaukee,+WI/Madison,+WI/@40.5504662,-89.1782838,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!1m5!1m1!1s0x884f2cce88145d39:0x7661a84704c91b0b!2m2!1d-81.6326234!2d38.3498195!1m5!1m1!1s0x883889c1b990de71:0xe43266f8cfb1b533!2m2!1d-82.9987942!2d39.9611755!1m5!1m1!1s0x884051b1de3821f9:0x69fb7e8be4c09317!2m2!1d-84.5120196!2d39.1031182!1m5!1m1!1s0x8842734c8b1953c9:0x536418a08867425c!2m2!1d-84.8732835!2d38.2009055!1m5!1m1!1s0x88690b1ab35bd511:0xd4d3b4282071fd32!2m2!1d-85.7584557!2d38.2526647!1m5!1m1!1s0x886b50ffa7796a03:0xd68e9df640b9ea7c!2m2!1d-86.158068!2d39.768403!1m5!1m1!1s0x880e2c3cd0f4cbed:0xafe0a6ad09c0c000!2m2!1d-87.6297982!2d41.8781136!1m5!1m1!1s0x880502d7578b47e7:0x445f1922b5417b84!2m2!1d-87.9064736!2d43.0389025!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Madison,+Wisconsin/Green+Bay,+WI/Mackinaw+City,+MI/Grand+Rapids,+MI/Lansing,+MI/Frankenmuth,+MI/Detroit,+MI/Cleveland,+OH/Pittsburgh,+PA/@43.1918863,-89.1853954,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x8806536d3a2019ff:0x4e0cfcb5ba484198!2m2!1d-89.4012302!2d43.0730517!1m5!1m1!1s0x8802e2e809b380f3:0x6370045214dcf571!2m2!1d-88.0132958!2d44.5133188!1m5!1m1!1s0x4d358b3940a9ad83:0xeac771ab20cc7a7a!2m2!1d-84.7271465!2d45.7774987!1m5!1m1!1s0x88185460bb502815:0xa593aacb1bd3a8d0!2m2!1d-85.6680863!2d42.9633599!1m5!1m1!1s0x8822c01c7f318c37:0x4378b62389029d9e!2m2!1d-84.5555347!2d42.732535!1m5!1m1!1s0x8823f287285df793:0x8050516199bcb01f!2m2!1d-83.7380194!2d43.331691!1m5!1m1!1s0x8824ca0110cb1d75:0x5776864e35b9c4d2!2m2!1d-83.0457538!2d42.331427!1m5!1m1!1s0x8830ef2ee3686b2d:0xed04cb55f7621842!2m2!1d-81.6943605!2d41.49932!1m5!1m1!1s0x8834f16f48068503:0x8df915a15aa21b34!2m2!1d-79.9958864!2d40.4406248!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/San+Juan,+Puerto+Rico/@28.406847,-80.5870322,5z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x8c03686fe268196f:0xad6b7f0f5c935adc!2m2!1d-66.1057355!2d18.4655394!3e4</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Washington+D.+C.,+DC/Honolulu,+HI/@24.8112769,-154.8564566,3z/data=!3m1!4b1!4m14!4m13!1m5!1m1!1s0x89b7c6de5af6e45b:0xc2524522d4885d2a!2m2!1d-77.0368707!2d38.9071923!1m5!1m1!1s0x7c00183b8cc3464d:0x4b28f55ff3a7976c!2m2!1d-157.8583333!2d21.3069444!3e4</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Orlando,+FL/Miami,+FL/Key+West,+FL/Everglades+City,+FL/Tampa,+FL/Tarpon+Springs,+FL/Tallahassee,+FL/Jacksonville,+FL/St.+Augustine,+FL/Orlando,+FL/@27.5091232,-84.4177219,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!1m5!1m1!1s0x88d9b0a20ec8c111:0xff96f271ddad4f65!2m2!1d-80.1917902!2d25.7616798!1m5!1m1!1s0x88d1b134ad952377:0x3fcee92f77463b5e!2m2!1d-81.7799871!2d24.5550593!1m5!1m1!1s0x88da5c605ba45fb1:0x92bcf49fb504533a!2m2!1d-81.3850695!2d25.8582443!1m5!1m1!1s0x88c2b782b3b9d1e1:0xa75f1389af96b463!2m2!1d-82.4571776!2d27.950575!1m5!1m1!1s0x88c28cfd6f0942df:0xf4297f0ce0bf24b7!2m2!1d-82.7567679!2d28.1461248!1m5!1m1!1s0x88ec8a5187124b53:0xebee077ad4fdb1f8!2m2!1d-84.2807329!2d30.4382559!1m5!1m1!1s0x88e5b716f1ceafeb:0xc4cd7d3896fcc7e2!2m2!1d-81.655651!2d30.3321838!1m5!1m1!1s0x88e6825775df7f4f:0xc2a183178b276027!2m2!1d-81.3124341!2d29.9012437!1m5!1m1!1s0x88e773d8fecdbc77:0xac3b2063ca5bf9e!2m2!1d-81.3789269!2d28.5383832!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Los+Angeles,+CA/Santa+Barbara,+CA/Solvang,+CA/San+Jose,+CA/San+Francisco,+CA/Sacramento,+CA/Reno,+NV/Virginia+City,+NV/Carson+City,+NV/Fresno,+CA/@36.7777641,-122.6363689,7z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!1m5!1m1!1s0x80e914c76f2d83d5:0xc8d13a64d7ba7648!2m2!1d-119.6981901!2d34.4208305!1m5!1m1!1s0x80e954a0fc922285:0x2d0e281b060bc156!2m2!1d-120.1376481!2d34.5958201!1m5!1m1!1s0x808fcae48af93ff5:0xb99d8c0aca9f717b!2m2!1d-121.8863286!2d37.3382082!1m5!1m1!1s0x80859a6d00690021:0x4a501367f076adff!2m2!1d-122.4194155!2d37.7749295!1m5!1m1!1s0x809ac672b28397f9:0x921f6aaa74197fdb!2m2!1d-121.4943996!2d38.5815719!1m5!1m1!1s0x809940ae9292a09d:0x40c5c5ce7438f787!2m2!1d-119.8138027!2d39.5296329!1m5!1m1!1s0x80990faad3daafd1:0x29dad257dc576fa9!2m2!1d-119.6499793!2d39.3095135!1m5!1m1!1s0x80990aa1f8deb471:0xf79c6c82bde23828!2m2!1d-119.7674034!2d39.1637984!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Fresno,+CA/Riverside,+CA/San+Diego,+CA/Los+Angeles,+CA/@34.7127545,-120.6716835,7z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x80945de1549e4e9d:0x7b12406449a3b811!2m2!1d-119.7871247!2d36.7377981!1m5!1m1!1s0x80dca6df7ff47dbb:0xf7a1d705135e0ae8!2m2!1d-117.3754942!2d33.9806005!1m5!1m1!1s0x80d9530fad921e4b:0xd3a21fdfd15df79!2m2!1d-117.1610838!2d32.715738!1m5!1m1!1s0x80c2c75ddc27da13:0xe22fdf6f254608f4!2m2!1d-118.2436849!2d34.0522342!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Phoenix,+AZ/Sedona,+AZ/Las+Vegas,+NV/St.+George,+UT/Taos,+NM/Santa+Fe,+NM/Albuquerque,+NM/Lubbock,+TX/El+Paso,+TX/Tucson,+AZ/@34.1501088,-117.508012,5z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!1m5!1m1!1s0x872da132f942b00d:0x5548c523fa6c8efd!2m2!1d-111.7609896!2d34.8697395!1m5!1m1!1s0x80beb782a4f57dd1:0x3accd5e6d5b379a3!2m2!1d-115.1398296!2d36.1699412!1m5!1m1!1s0x80ca44d0984939e5:0x531707f2f8a11c1e!2m2!1d-113.5684164!2d37.0965278!1m5!1m1!1s0x871764da7f11fcb1:0x90ea918361a9b782!2m2!1d-105.5733788!2d36.4072134!1m5!1m1!1s0x87185043e79852a9:0x8c902373fd88df40!2m2!1d-105.937799!2d35.6869752!1m5!1m1!1s0x87220addd309837b:0xc0d3f8ceb8d9f6fd!2m2!1d-106.650422!2d35.0843859!1m5!1m1!1s0x86fe12add37ddd39:0x1af0042922e84287!2m2!1d-101.8551665!2d33.5778631!1m5!1m1!1s0x86e73f8bc5fe3b69:0xe39184e3ab9d0222!2m2!1d-106.4850217!2d31.7618778!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Tucson,+AZ/Phoenix,+AZ/@32.6659365,-112.3105217,7.68z/data=!4m17!4m16!1m5!1m1!1s0x86d665410b2ced2b:0x73c32d384d16c715!2m2!1d-110.9747108!2d32.2226066!1m5!1m1!1s0x872b12ed50a179cb:0x8c69c7f8354a1bac!2m2!1d-112.0740373!2d33.4483771!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Dallas,+TX/Austin,+TX/San+Antonio,+TX/McAllen,+TX/Houston,+TX/Baton+Rouge,+LA/New+Orleans,+LA/Gulfport,+MS/Jackson,+MS/@29.4197283,-98.2903561,6z/data=!3m1!4b1!4m59!4m58!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!1m5!1m1!1s0x8644b599a0cc032f:0x5d9b464bd469d57a!2m2!1d-97.7430608!2d30.267153!1m5!1m1!1s0x865c58af04d00eaf:0x856e13b10a016bc!2m2!1d-98.4936282!2d29.4241219!1m5!1m1!1s0x866576324d9637df:0x2f1d39a9b52c0eb8!2m2!1d-98.2300124!2d26.2034071!1m5!1m1!1s0x8640b8b4488d8501:0xca0d02def365053b!2m2!1d-95.3698028!2d29.7604267!1m5!1m1!1s0x86243867325f74cb:0x2123f1db91579a1d!2m2!1d-91.1871466!2d30.4514677!1m5!1m1!1s0x8620a454b2118265:0xdb065be85e22d3b4!2m2!1d-90.0715323!2d29.9510658!1m5!1m1!1s0x889c166ee80114e5:0xc2614d446e819544!2m2!1d-89.0928155!2d30.3674198!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Jackson,+MS/Little+Rock,+AR/Fayetteville,+AR/Dallas,+TX/@32.5477822,-99.0081422,5.75z/data=!4m29!4m28!1m5!1m1!1s0x86282b7f90741b21:0x713cde441f038a0!2m2!1d-90.1848103!2d32.2987573!1m5!1m1!1s0x87d2a134a11f569b:0x3405f5100df35b17!2m2!1d-92.2895948!2d34.7464809!1m5!1m1!1s0x87c96f7b2fb53e9d:0x4519f069fcb4c8cf!2m2!1d-94.157853!2d36.0662419!1m5!1m1!1s0x864c19f77b45974b:0xb9ec9ba4f647678f!2m2!1d-96.7969879!2d32.7766642!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>lon</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Atlanta,+GA/Helen,+GA/Nashville,+TN/Knoxville,+TN/Charlotte,+NC/Greensboro,+NC/Raleigh,+NC/Columbia,+SC/Charleston,+SC/Savannah,+GA/@34.0640266,-87.1468938,6z/data=!3m1!4b1!4m65!4m64!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!1m5!1m1!1s0x885f37d40b3a2aa1:0x8ed537fed96523a8!2m2!1d-83.7315675!2d34.7014839!1m5!1m1!1s0x8864ec3213eb903d:0x7d3fb9d0a1e9daa0!2m2!1d-86.7816016!2d36.1626638!1m5!1m1!1s0x885c162246ce42a9:0x7bea92dac4f534c5!2m2!1d-83.9207392!2d35.9606384!1m5!1m1!1s0x88541fc4fc381a81:0x884650e6bf43d164!2m2!1d-80.8431267!2d35.2270869!1m5!1m1!1s0x8853193f38c77b79:0x93b9c49478be12c8!2m2!1d-79.7919754!2d36.0726354!1m5!1m1!1s0x89ac5a2f9f51e0f7:0x6790b6528a11f0ad!2m2!1d-78.6381787!2d35.7795897!1m5!1m1!1s0x88f8a5697931d1e3:0xf32808f4b379fa96!2m2!1d-81.0348144!2d34.0007104!1m5!1m1!1s0x88fe7a42dca82477:0x35faf7e0aee1ec6b!2m2!1d-79.9310512!2d32.7764749!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/dir/Savannah,+GA/Montgomery,+AL/Birmingham,+AL/Atlanta,+GA/@32.8510822,-88.4506539,6z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!1m5!1m1!1s0x888e8194b0d481f9:0x8e1b511d354285ff!2m2!1d-86.3077368!2d32.3792233!1m5!1m1!1s0x888911df5885bfd3:0x25507409eaba54ce!2m2!1d-86.8103567!2d33.5185892!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!2m1!2b1!3e0!4e1</t>
-  </si>
-  <si>
-    <t>Northeast + MD, DE, VA</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>SEA &gt; ANC</t>
-  </si>
-  <si>
-    <t>SFO &gt; HNL</t>
-  </si>
-  <si>
-    <t>DC Two Hour Radius</t>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Mar</t>
   </si>
 </sst>
 </file>
@@ -3203,11 +3191,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A135" sqref="A135"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3216,8 +3204,8 @@
     <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -3245,10 +3233,10 @@
         <v>152</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -4782,11 +4770,11 @@
         <v>1</v>
       </c>
       <c r="F51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" s="1">
         <v>-90.071532300000001</v>
@@ -5281,7 +5269,7 @@
         <v>0</v>
       </c>
       <c r="G67" s="12">
-        <f t="shared" ref="G67:G130" si="3">((1-E67)-(1-F67))+((1-F67)*2)</f>
+        <f t="shared" ref="G67:G129" si="3">((1-E67)-(1-F67))+((1-F67)*2)</f>
         <v>1</v>
       </c>
       <c r="H67" s="1">
@@ -6539,7 +6527,7 @@
         <v>78</v>
       </c>
       <c r="C108" s="2" t="str">
-        <f t="shared" ref="C108:C134" si="5">RIGHT(B108,2)</f>
+        <f t="shared" ref="C108:C129" si="5">RIGHT(B108,2)</f>
         <v>TX</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -7211,161 +7199,6 @@
       </c>
       <c r="I129" s="1">
         <v>41.139981400000003</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A130" s="2">
-        <v>130</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C130" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>DC</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E130" s="1">
-        <v>1</v>
-      </c>
-      <c r="F130" s="1">
-        <v>1</v>
-      </c>
-      <c r="G130" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H130" s="1">
-        <v>-77.036870699999994</v>
-      </c>
-      <c r="I130" s="1">
-        <v>38.907192299999998</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A131" s="2">
-        <v>131</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C131" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>MD</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E131" s="1">
-        <v>1</v>
-      </c>
-      <c r="F131" s="1">
-        <v>1</v>
-      </c>
-      <c r="G131" s="1">
-        <f t="shared" ref="G131:G134" si="6">((1-E131)-(1-F131))+((1-F131)*2)</f>
-        <v>0</v>
-      </c>
-      <c r="H131" s="1">
-        <v>-76.492182900000003</v>
-      </c>
-      <c r="I131" s="1">
-        <v>38.978445299999997</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A132" s="4">
-        <v>132</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C132" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>MD</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E132" s="5">
-        <v>1</v>
-      </c>
-      <c r="F132" s="5">
-        <v>0</v>
-      </c>
-      <c r="G132" s="5">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="H132" s="1">
-        <v>-76.612189299999997</v>
-      </c>
-      <c r="I132" s="1">
-        <v>39.290384799999998</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A133" s="4">
-        <v>133</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C133" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>DE</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E133" s="5">
-        <v>0</v>
-      </c>
-      <c r="F133" s="5">
-        <v>0</v>
-      </c>
-      <c r="G133" s="5">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="H133" s="1">
-        <v>-75.524368199999998</v>
-      </c>
-      <c r="I133" s="1">
-        <v>39.158168000000003</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A134" s="2">
-        <v>134</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C134" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>PA</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E134" s="1">
-        <v>1</v>
-      </c>
-      <c r="F134" s="1">
-        <v>1</v>
-      </c>
-      <c r="G134" s="1">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H134" s="1">
-        <v>-76.8867008</v>
-      </c>
-      <c r="I134" s="1">
-        <v>40.273191099999998</v>
       </c>
     </row>
   </sheetData>
@@ -7383,10 +7216,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7401,10 +7234,12 @@
     <col min="8" max="10" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>235</v>
       </c>
@@ -7418,192 +7253,205 @@
         <v>234</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>237</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>276</v>
       </c>
       <c r="C2" s="1">
-        <v>1056</v>
+        <v>719</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" ref="D2:D16" si="0">IF(B2="Drive",0,2)+_xlfn.CEILING.MATH(C2/200,1)+K2</f>
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="K2" s="1">
+        <f>(3*2)+3-2</f>
+        <v>7</v>
+      </c>
+      <c r="L2" s="1">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1056</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E3" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="H3" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="K3" s="1">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="L2" s="1">
-        <v>6</v>
-      </c>
-      <c r="M2" s="1">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C3" s="1">
-        <v>719</v>
-      </c>
-      <c r="D3" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="K3" s="1">
-        <f>(3*2)+3-2</f>
+      <c r="L3" s="1">
         <v>7</v>
       </c>
-      <c r="L3" s="1">
-        <v>6</v>
-      </c>
       <c r="M3" s="1">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C4" s="1">
-        <v>2211</v>
+        <v>1610</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="E4" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
       </c>
       <c r="L4" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M4" s="1">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="N4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="C5" s="1">
-        <v>1610</v>
+        <f>1097+1202+(237*2)</f>
+        <v>2773</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -7614,8 +7462,11 @@
       <c r="M5" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>141</v>
       </c>
@@ -7629,120 +7480,128 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>241</v>
+      <c r="E6" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>220</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
       </c>
       <c r="L6" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M6" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>206</v>
+        <v>143</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>286</v>
+        <v>224</v>
       </c>
       <c r="C7" s="1">
-        <v>2403</v>
+        <v>2211</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>250</v>
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>269</v>
+        <v>213</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>251</v>
       </c>
       <c r="K7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="1">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="M7" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="N7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C8" s="1">
-        <f>1097+1202+(237*2)</f>
-        <v>2773</v>
+        <v>2403</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>243</v>
+      <c r="E8" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>270</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>271</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>262</v>
+        <v>274</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>258</v>
       </c>
       <c r="K8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M8" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="N8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>135</v>
       </c>
@@ -7756,11 +7615,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>243</v>
+      <c r="E9" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>218</v>
@@ -7772,13 +7631,16 @@
         <v>0</v>
       </c>
       <c r="L9" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M9" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>140</v>
       </c>
@@ -7793,23 +7655,23 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>243</v>
+      <c r="E10" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>221</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -7818,84 +7680,90 @@
         <v>5</v>
       </c>
       <c r="M10" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="N10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" s="1">
+        <f>1951+(278*2)</f>
+        <v>2507</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>5</v>
+      </c>
+      <c r="M11" s="1">
+        <v>11</v>
+      </c>
+      <c r="N11" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <f>2228+113</f>
         <v>2341</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E12" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="J12" s="23" t="s">
         <v>251</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>278</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="M11" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" s="1">
-        <f>1951+(278*2)</f>
-        <v>2507</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>262</v>
       </c>
       <c r="K12" s="1">
         <v>0</v>
@@ -7904,10 +7772,13 @@
         <v>4</v>
       </c>
       <c r="M12" s="1">
+        <v>11</v>
+      </c>
+      <c r="N12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>137</v>
       </c>
@@ -7922,160 +7793,172 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>252</v>
+      <c r="E13" s="1" t="s">
+        <v>283</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>216</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="K13" s="1">
         <v>0</v>
       </c>
       <c r="L13" s="1">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M13" s="1">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>212</v>
+        <v>277</v>
       </c>
       <c r="C14" s="1">
-        <v>1384</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>253</v>
+      <c r="E14" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>248</v>
+        <v>284</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J14" s="23"/>
       <c r="K14" s="1">
-        <v>0</v>
+        <f>(3*2)+3-2</f>
+        <v>7</v>
       </c>
       <c r="L14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M14" s="1">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="N14" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>288</v>
+        <v>232</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>254</v>
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>238</v>
+        <v>284</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J15" s="23"/>
       <c r="K15" s="1">
-        <f>(3*2)+3-2</f>
-        <v>7</v>
+        <f>(1*2)+3-2</f>
+        <v>3</v>
       </c>
       <c r="L15" s="1">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="M15" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="N15" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>223</v>
+        <v>131</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>1384</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>254</v>
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>238</v>
+        <v>284</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="J16" s="23"/>
       <c r="K16" s="1">
-        <f>(1*2)+3-2</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L16" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="M16" s="1">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="N16" s="1">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L16">
-    <sortCondition ref="L2:L16"/>
-    <sortCondition descending="1" ref="K2:K16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N16">
+    <sortCondition ref="M2:M16"/>
+    <sortCondition descending="1" ref="L2:L16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Begin draft #2 (D2) of travel_weather project code
</commit_message>
<xml_diff>
--- a/A_Input/city_list.xlsx
+++ b/A_Input/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/us_travels/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B413607E-1851-4445-B105-41B491D9EE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2B2A14-F299-C045-AFD9-D5B0424D05AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34280" yWindow="2120" windowWidth="23380" windowHeight="15340" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-38040" yWindow="-1780" windowWidth="21560" windowHeight="17320" activeTab="1" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -864,9 +864,6 @@
     <t>https://www.google.com/maps/dir/Savannah,+GA/Montgomery,+AL/Birmingham,+AL/Atlanta,+GA/@32.8510822,-88.4506539,6z/data=!3m1!4b1!4m29!4m28!1m5!1m1!1s0x88fb75fc78f20659:0x4e0c6751036020bc!2m2!1d-81.091203!2d32.0808989!1m5!1m1!1s0x888e8194b0d481f9:0x8e1b511d354285ff!2m2!1d-86.3077368!2d32.3792233!1m5!1m1!1s0x888911df5885bfd3:0x25507409eaba54ce!2m2!1d-86.8103567!2d33.5185892!1m5!1m1!1s0x88f5045d6993098d:0x66fede2f990b630b!2m2!1d-84.3879824!2d33.7489954!2m1!2b1!3e0!4e1</t>
   </si>
   <si>
-    <t>Northeast + MD, DE, VA</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -898,6 +895,9 @@
   </si>
   <si>
     <t>Mar</t>
+  </si>
+  <si>
+    <t>Northeast + DC, DE, MD, VA</t>
   </si>
 </sst>
 </file>
@@ -3193,9 +3193,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4038DB3-8426-7C4B-9410-FFCEAF90185D}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4040,28 +4040,28 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="4" t="str">
+      <c r="C28" s="2" t="str">
         <f t="shared" si="1"/>
         <v>DE</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E28" s="5">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0</v>
-      </c>
-      <c r="G28" s="5">
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H28" s="1">
         <v>-75.524368199999998</v>
@@ -7218,8 +7218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9631FB04-418B-8B42-963F-59DBC5B62716}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7280,7 +7280,7 @@
         <v>245</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -7288,7 +7288,7 @@
         <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" s="1">
         <v>719</v>
@@ -7298,7 +7298,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>241</v>
@@ -7344,7 +7344,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>241</v>
@@ -7390,7 +7390,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>241</v>
@@ -7425,7 +7425,7 @@
         <v>132</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C5" s="1">
         <f>1097+1202+(237*2)</f>
@@ -7481,7 +7481,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>239</v>
@@ -7561,7 +7561,7 @@
         <v>206</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C8" s="1">
         <v>2403</v>
@@ -7577,7 +7577,7 @@
         <v>239</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="H8" s="24" t="s">
         <v>256</v>
@@ -7656,10 +7656,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>221</v>
@@ -7691,7 +7691,7 @@
         <v>130</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C11" s="1">
         <f>1951+(278*2)</f>
@@ -7702,10 +7702,10 @@
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>215</v>
@@ -7748,10 +7748,10 @@
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>219</v>
@@ -7794,7 +7794,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>238</v>
@@ -7829,7 +7829,7 @@
         <v>222</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -7839,10 +7839,10 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>164</v>
@@ -7883,10 +7883,10 @@
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>192</v>
@@ -7927,10 +7927,10 @@
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>162</v>

</xml_diff>